<commit_message>
try without either ethnic or hearing merge
</commit_message>
<xml_diff>
--- a/output/multivariated_linear.xlsx
+++ b/output/multivariated_linear.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t xml:space="preserve">Characteristic
 </t>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">     Chinese</t>
   </si>
   <si>
+    <t xml:space="preserve">     others</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marital status</t>
   </si>
   <si>
@@ -63,9 +66,6 @@
     <t xml:space="preserve">     Bangkok</t>
   </si>
   <si>
-    <t xml:space="preserve">     others</t>
-  </si>
-  <si>
     <t xml:space="preserve">Education</t>
   </si>
   <si>
@@ -138,7 +138,10 @@
     <t xml:space="preserve">     Gait aid</t>
   </si>
   <si>
-    <t xml:space="preserve">PatientHearing</t>
+    <t xml:space="preserve">Hearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Hearing aid</t>
   </si>
   <si>
     <t xml:space="preserve">     Hearing impairment</t>
@@ -296,146 +299,158 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">-0.02, 0.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.55, 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.05, 0.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.7, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.50, 0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.41, 2.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.78, 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.94, 0.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.0, 3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.8, 3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.75, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.4, 0.88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.56, 0.74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.96, 0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.5, 0.56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.3, 0.70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.5, 0.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.66, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.48, 1.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.0, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.8, 0.87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.20, 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.87, 0.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.5, 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.88, 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.69, 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.2, 4.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.1, 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.69, 2.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.30, 0.82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.1, 5.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.12, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.3, 6.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.0, 2.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.8, 1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7.3, 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.45, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.92, 0.44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.80, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.29, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.51, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.51, 0.79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.24, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.55, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09, 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.52, 2.8</t>
+    <t xml:space="preserve">-0.03, 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.31, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.05, 0.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.6, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.3, 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.52, 0.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.44, 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.73, 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.93, 0.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.9, 3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.6, 3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.7, 3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.1, 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.3, 0.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.58, 0.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.0, 0.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.6, 0.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.3, 0.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.6, 0.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.49, 1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.70, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.96, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.6, 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.6, 3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.04, 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.77, 0.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.3, 1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.60, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.63, 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.72, 4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.1, 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.71, 2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.21, 0.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.84, 5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.16, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.8, 6.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5.8, 2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-6.5, 1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-6.9, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.40, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.91, 0.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.83, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.45, 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.37, 0.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.43, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00, 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.09, 2.2</t>
   </si>
   <si>
     <t xml:space="preserve">p-value
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;0.001</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;0.9</t>
@@ -889,13 +904,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -903,13 +918,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -917,13 +932,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -931,13 +946,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -945,13 +960,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="n">
-        <v>0.29</v>
+        <v>0.51</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
@@ -962,7 +977,7 @@
         <v>0.02</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>0.5</v>
@@ -973,13 +988,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -987,13 +1002,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -1001,27 +1016,27 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="n">
-        <v>-0.16</v>
+        <v>-0.1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>90</v>
+      <c r="B10" s="8" t="n">
+        <v>9.7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1035,21 +1050,21 @@
         <v>91</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="n">
-        <v>0.22</v>
+      <c r="B12" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="8" t="n">
-        <v>0.5</v>
+        <v>92</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1057,13 +1072,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="n">
-        <v>1.1</v>
+        <v>0.18</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D13" s="8" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1071,27 +1086,27 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="n">
-        <v>0.16</v>
+        <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D14" s="8" t="n">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>90</v>
+      <c r="B15" s="8" t="n">
+        <v>0.17</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1105,40 +1120,40 @@
         <v>91</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="n">
-        <v>-0.38</v>
+      <c r="B17" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="8" t="n">
-        <v>0.2</v>
+        <v>92</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>90</v>
+        <v>9</v>
+      </c>
+      <c r="B18" s="8" t="n">
+        <v>-0.38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>91</v>
@@ -1147,68 +1162,68 @@
         <v>91</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="n">
-        <v>0.68</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="8" t="n">
-        <v>0.6</v>
+        <v>92</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8" t="n">
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D21" s="8" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="8" t="n">
-        <v>0.67</v>
+        <v>0.99</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D22" s="8" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>90</v>
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="n">
+        <v>0.8</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="D23" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>91</v>
@@ -1217,68 +1232,68 @@
         <v>91</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="8" t="n">
-        <v>0.4</v>
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="8" t="n">
-        <v>0.5</v>
+        <v>92</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8" t="n">
-        <v>-0.24</v>
+        <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="8" t="n">
-        <v>0.7</v>
+        <v>106</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="8" t="n">
-        <v>0.09</v>
+        <v>-0.21</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D27" s="8" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>90</v>
+        <v>26</v>
+      </c>
+      <c r="B28" s="8" t="n">
+        <v>0.05</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>90</v>
+        <v>108</v>
+      </c>
+      <c r="D28" s="8" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>91</v>
@@ -1287,82 +1302,82 @@
         <v>91</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="8" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="8" t="n">
-        <v>-0.48</v>
+        <v>-0.09</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D31" s="8" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="8" t="n">
-        <v>-0.27</v>
+        <v>-0.57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D32" s="8" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="8" t="n">
-        <v>-0.58</v>
+        <v>-0.35</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D33" s="8" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>90</v>
+        <v>32</v>
+      </c>
+      <c r="B34" s="8" t="n">
+        <v>-0.76</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>90</v>
+        <v>112</v>
+      </c>
+      <c r="D34" s="8" t="n">
+        <v>0.095</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>91</v>
@@ -1371,68 +1386,68 @@
         <v>91</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="8" t="n">
-        <v>0.44</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="8" t="n">
-        <v>0.4</v>
+        <v>92</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="8" t="n">
-        <v>0.69</v>
+        <v>0.58</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D37" s="8" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="8" t="n">
-        <v>0.33</v>
+        <v>0.44</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D38" s="8" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>90</v>
+        <v>37</v>
+      </c>
+      <c r="B39" s="8" t="n">
+        <v>0.32</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>90</v>
+        <v>115</v>
+      </c>
+      <c r="D39" s="8" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>91</v>
@@ -1441,40 +1456,40 @@
         <v>91</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" ht="NA" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="8" t="n">
-        <v>-0.49</v>
+        <v>39</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="8" t="n">
-        <v>0.5</v>
+        <v>92</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>90</v>
+        <v>40</v>
+      </c>
+      <c r="B42" s="8" t="n">
+        <v>-0.21</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>90</v>
+        <v>116</v>
+      </c>
+      <c r="D42" s="8" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="43" ht="NA" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>91</v>
@@ -1483,824 +1498,852 @@
         <v>91</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" ht="NA" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="8" t="n">
-        <v>0.99</v>
+        <v>39</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="8" t="n">
-        <v>0.1</v>
+        <v>92</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="45" ht="NA" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>90</v>
+        <v>42</v>
+      </c>
+      <c r="B45" s="8" t="n">
+        <v>-0.34</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>90</v>
+        <v>117</v>
+      </c>
+      <c r="D45" s="8" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="46" ht="NA" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>91</v>
+        <v>43</v>
+      </c>
+      <c r="B46" s="8" t="n">
+        <v>1.1</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>90</v>
+        <v>118</v>
+      </c>
+      <c r="D46" s="8" t="n">
+        <v>0.058</v>
       </c>
     </row>
     <row r="47" ht="NA" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="8" t="n">
-        <v>-0.3</v>
+      <c r="B47" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="8" t="n">
-        <v>0.3</v>
+        <v>91</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="48" ht="NA" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" ht="NA" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>91</v>
+        <v>45</v>
+      </c>
+      <c r="B49" s="8" t="n">
+        <v>-0.22</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>90</v>
+        <v>119</v>
+      </c>
+      <c r="D49" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="50" ht="NA" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="8" t="n">
-        <v>-0.53</v>
+        <v>46</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" s="8" t="n">
-        <v>0.6</v>
+        <v>91</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="51" ht="NA" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" s="8" t="n">
-        <v>0.17</v>
+        <v>47</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D51" s="8" t="n">
-        <v>0.8</v>
+        <v>92</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="52" ht="NA" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>90</v>
+        <v>48</v>
+      </c>
+      <c r="B52" s="8" t="n">
+        <v>-0.28</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="D52" s="8" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="53" ht="NA" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>91</v>
+        <v>49</v>
+      </c>
+      <c r="B53" s="8" t="n">
+        <v>0.41</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>90</v>
+        <v>121</v>
+      </c>
+      <c r="D53" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="54" ht="NA" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="8" t="n">
-        <v>0.4</v>
+        <v>50</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="8" t="n">
-        <v>0.5</v>
+        <v>91</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="55" ht="NA" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="8" t="n">
-        <v>1.4</v>
+        <v>51</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" s="8" t="n">
-        <v>0.3</v>
+        <v>92</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="56" ht="NA" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>90</v>
+        <v>52</v>
+      </c>
+      <c r="B56" s="8" t="n">
+        <v>0.43</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>90</v>
+        <v>122</v>
+      </c>
+      <c r="D56" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="57" ht="NA" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>91</v>
+        <v>53</v>
+      </c>
+      <c r="B57" s="8" t="n">
+        <v>1.8</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>90</v>
+        <v>123</v>
+      </c>
+      <c r="D57" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="58" ht="NA" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="8" t="n">
-        <v>0.52</v>
+        <v>54</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D58" s="8" t="n">
-        <v>0.5</v>
+        <v>91</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="59" ht="NA" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" s="8" t="n">
-        <v>1.1</v>
+        <v>55</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D59" s="8" t="n">
-        <v>0.2</v>
+        <v>92</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="60" ht="NA" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>90</v>
+        <v>56</v>
+      </c>
+      <c r="B60" s="8" t="n">
+        <v>0.46</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>90</v>
+        <v>124</v>
+      </c>
+      <c r="D60" s="8" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="61" ht="NA" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>91</v>
+        <v>57</v>
+      </c>
+      <c r="B61" s="8" t="n">
+        <v>1</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D61" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="62" ht="NA" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="8" t="n">
-        <v>0.26</v>
+      <c r="B62" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" s="8" t="n">
-        <v>0.4</v>
+        <v>91</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="63" ht="NA" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="8" t="n">
-        <v>2.3</v>
+        <v>39</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="8" t="n">
-        <v>0.2</v>
+        <v>92</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="64" ht="NA" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" s="8" t="n">
-        <v>0.69</v>
+        <v>0.33</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D64" s="8" t="n">
-        <v>0.018</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="65" ht="NA" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>90</v>
+        <v>60</v>
+      </c>
+      <c r="B65" s="8" t="n">
+        <v>2.5</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>90</v>
+        <v>127</v>
+      </c>
+      <c r="D65" s="8" t="n">
+        <v>0.14</v>
       </c>
     </row>
     <row r="66" ht="NA" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>91</v>
+        <v>61</v>
+      </c>
+      <c r="B66" s="8" t="n">
+        <v>0.73</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>90</v>
+        <v>128</v>
+      </c>
+      <c r="D66" s="8" t="n">
+        <v>0.013</v>
       </c>
     </row>
     <row r="67" ht="NA" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" s="8" t="n">
-        <v>1.6</v>
+        <v>62</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D67" s="8" t="n">
-        <v>0.5</v>
+        <v>91</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="68" ht="NA" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="8" t="n">
-        <v>-1.7</v>
+        <v>63</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D68" s="8" t="n">
-        <v>0.4</v>
+        <v>92</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="69" ht="NA" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B69" s="8" t="n">
-        <v>-2.5</v>
+        <v>1.9</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D69" s="8" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="70" ht="NA" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B70" s="8" t="n">
-        <v>-2.9</v>
+        <v>-1.7</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D70" s="8" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="71" ht="NA" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>90</v>
+        <v>66</v>
+      </c>
+      <c r="B71" s="8" t="n">
+        <v>-2.3</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>90</v>
+        <v>131</v>
+      </c>
+      <c r="D71" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="72" ht="NA" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>91</v>
+        <v>67</v>
+      </c>
+      <c r="B72" s="8" t="n">
+        <v>-2.7</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>90</v>
+        <v>132</v>
+      </c>
+      <c r="D72" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="73" ht="NA" customHeight="1">
       <c r="A73" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="8" t="n">
-        <v>0.45</v>
+        <v>68</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D73" s="8" t="n">
-        <v>0.3</v>
+        <v>91</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="74" ht="NA" customHeight="1">
       <c r="A74" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" ht="NA" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>91</v>
+        <v>70</v>
+      </c>
+      <c r="B75" s="8" t="n">
+        <v>0.46</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>90</v>
+        <v>133</v>
+      </c>
+      <c r="D75" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="76" ht="NA" customHeight="1">
       <c r="A76" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B76" s="8" t="n">
-        <v>-0.24</v>
+      <c r="B76" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="8" t="n">
-        <v>0.5</v>
+        <v>91</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="77" ht="NA" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" ht="NA" customHeight="1">
       <c r="A78" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>91</v>
+        <v>72</v>
+      </c>
+      <c r="B78" s="8" t="n">
+        <v>-0.25</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>90</v>
+        <v>134</v>
+      </c>
+      <c r="D78" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="79" ht="NA" customHeight="1">
       <c r="A79" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B79" s="8" t="n">
-        <v>0.29</v>
+      <c r="B79" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D79" s="8" t="n">
-        <v>0.6</v>
+        <v>91</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="80" ht="NA" customHeight="1">
       <c r="A80" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" ht="NA" customHeight="1">
       <c r="A81" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>91</v>
+        <v>74</v>
+      </c>
+      <c r="B81" s="8" t="n">
+        <v>0.22</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>90</v>
+        <v>135</v>
+      </c>
+      <c r="D81" s="8" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="82" ht="NA" customHeight="1">
       <c r="A82" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="8" t="n">
-        <v>0.96</v>
+      <c r="B82" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D82" s="8" t="n">
-        <v>0.005</v>
+        <v>91</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="83" ht="NA" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" ht="NA" customHeight="1">
       <c r="A84" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>91</v>
+        <v>76</v>
+      </c>
+      <c r="B84" s="8" t="n">
+        <v>0.76</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>90</v>
+        <v>136</v>
+      </c>
+      <c r="D84" s="8" t="n">
+        <v>0.023</v>
       </c>
     </row>
     <row r="85" ht="NA" customHeight="1">
       <c r="A85" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="8" t="n">
-        <v>0.52</v>
+      <c r="B85" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D85" s="8" t="n">
-        <v>0.3</v>
+        <v>91</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="86" ht="NA" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" ht="NA" customHeight="1">
       <c r="A87" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>91</v>
+        <v>78</v>
+      </c>
+      <c r="B87" s="8" t="n">
+        <v>0.55</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="D87" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="88" ht="NA" customHeight="1">
       <c r="A88" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B88" s="8" t="n">
-        <v>0.14</v>
+      <c r="B88" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D88" s="8" t="n">
-        <v>0.7</v>
+        <v>91</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="89" ht="NA" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" ht="NA" customHeight="1">
       <c r="A90" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="B90" s="8" t="n">
+        <v>0.26</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>90</v>
+        <v>138</v>
+      </c>
+      <c r="D90" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="91" ht="NA" customHeight="1">
       <c r="A91" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B91" s="8" t="n">
-        <v>0.82</v>
+      <c r="B91" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D91" s="8" t="n">
-        <v>0.006</v>
+        <v>91</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="92" ht="NA" customHeight="1">
       <c r="A92" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" ht="NA" customHeight="1">
       <c r="A93" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>91</v>
+        <v>82</v>
+      </c>
+      <c r="B93" s="8" t="n">
+        <v>0.81</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>90</v>
+        <v>139</v>
+      </c>
+      <c r="D93" s="8" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="94" ht="NA" customHeight="1">
       <c r="A94" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B94" s="8" t="n">
-        <v>0.4</v>
+      <c r="B94" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D94" s="8" t="n">
-        <v>0.4</v>
+        <v>91</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="95" ht="NA" customHeight="1">
       <c r="A95" s="3" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" ht="NA" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="B96" s="8" t="n">
+        <v>0.48</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>90</v>
+        <v>140</v>
+      </c>
+      <c r="D96" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="97" ht="NA" customHeight="1">
       <c r="A97" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B97" s="8" t="n">
-        <v>0.52</v>
+      <c r="B97" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D97" s="8" t="n">
-        <v>0.1</v>
+        <v>91</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="98" ht="NA" customHeight="1">
       <c r="A98" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" ht="NA" customHeight="1">
       <c r="A99" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
+      </c>
+      <c r="B99" s="8" t="n">
+        <v>0.59</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>90</v>
+        <v>141</v>
+      </c>
+      <c r="D99" s="8" t="n">
+        <v>0.052</v>
       </c>
     </row>
     <row r="100" ht="NA" customHeight="1">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B100" s="9" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D100" s="9" t="n">
-        <v>0.005</v>
+      <c r="B100" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="101" ht="NA" customHeight="1">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="102" ht="NA" customHeight="1">
+      <c r="A102" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>88</v>
+      <c r="B102" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" s="9" t="n">
+        <v>0.071</v>
+      </c>
+    </row>
+    <row r="103" ht="NA" customHeight="1">
+      <c r="A103" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A103:D103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
1.remove row 66 2.make beautiful plot
</commit_message>
<xml_diff>
--- a/output/multivariated_linear.xlsx
+++ b/output/multivariated_linear.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t xml:space="preserve">Characteristic
 </t>
@@ -42,30 +42,30 @@
     <t xml:space="preserve">     Chinese</t>
   </si>
   <si>
+    <t xml:space="preserve">Marital status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     married</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     divorced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     widow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Bangkok</t>
+  </si>
+  <si>
     <t xml:space="preserve">     others</t>
   </si>
   <si>
-    <t xml:space="preserve">Marital status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     married</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     divorced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     widow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Bangkok</t>
-  </si>
-  <si>
     <t xml:space="preserve">Education</t>
   </si>
   <si>
@@ -138,10 +138,7 @@
     <t xml:space="preserve">     Gait aid</t>
   </si>
   <si>
-    <t xml:space="preserve">Hearing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Hearing aid</t>
+    <t xml:space="preserve">PatientHearing</t>
   </si>
   <si>
     <t xml:space="preserve">     Hearing impairment</t>
@@ -299,158 +296,146 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">-0.03, 0.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.31, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.05, 0.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.6, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.3, 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.52, 0.88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.44, 2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.73, 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.93, 0.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.9, 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.6, 3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.7, 3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.1, 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.3, 0.88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.58, 0.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.0, 0.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.6, 0.44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.3, 0.61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.6, 0.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.49, 1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.70, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.96, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.6, 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.6, 3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.04, 2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.77, 0.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.3, 1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.60, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.63, 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.72, 4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.1, 2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.71, 2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.21, 0.88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.84, 5.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.16, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.8, 6.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.8, 2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.5, 1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-6.9, 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.40, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.91, 0.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.83, 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.11, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.45, 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.37, 0.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.25, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.43, 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00, 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.09, 2.2</t>
+    <t xml:space="preserve">-0.02, 0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.55, 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.05, 0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.7, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.50, 0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.41, 2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.78, 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.94, 0.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.0, 3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.8, 3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.75, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.4, 0.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.56, 0.74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.96, 0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.5, 0.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.3, 0.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.5, 0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.66, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.48, 1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.0, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.8, 0.87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.20, 2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.87, 0.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.5, 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.88, 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.69, 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.2, 4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.1, 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.69, 2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.30, 0.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.1, 5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.12, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.3, 6.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-6.0, 2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-6.8, 1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-7.3, 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.45, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.92, 0.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.80, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.29, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.51, 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.51, 0.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.24, 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.55, 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.09, 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52, 2.8</t>
   </si>
   <si>
     <t xml:space="preserve">p-value
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;0.001</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;0.9</t>
@@ -904,13 +889,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -918,13 +903,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
@@ -932,13 +917,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" ht="NA" customHeight="1">
@@ -946,13 +931,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
@@ -960,13 +945,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="n">
-        <v>0.51</v>
+        <v>0.29</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
@@ -977,7 +962,7 @@
         <v>0.02</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>0.5</v>
@@ -988,13 +973,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
@@ -1002,13 +987,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -1016,27 +1001,27 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="n">
-        <v>-0.1</v>
+        <v>-0.16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="n">
-        <v>9.7</v>
+      <c r="B10" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -1050,21 +1035,21 @@
         <v>91</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>92</v>
+      <c r="B12" s="8" t="n">
+        <v>0.22</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>91</v>
+        <v>97</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
@@ -1072,13 +1057,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="n">
-        <v>0.18</v>
+        <v>1.1</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="8" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -1086,27 +1071,27 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="n">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="8" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="n">
-        <v>0.17</v>
+      <c r="B15" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="8" t="n">
-        <v>0.7</v>
+        <v>90</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1120,40 +1105,40 @@
         <v>91</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>92</v>
+      <c r="B17" s="8" t="n">
+        <v>-0.38</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>91</v>
+        <v>100</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="8" t="n">
-        <v>-0.38</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="8" t="n">
-        <v>0.2</v>
+        <v>90</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>91</v>
@@ -1162,68 +1147,68 @@
         <v>91</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>92</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="n">
+        <v>0.68</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" ht="NA" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="8" t="n">
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="8" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="8" t="n">
-        <v>0.99</v>
+        <v>0.67</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D22" s="8" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="8" t="n">
-        <v>0.8</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="8" t="n">
-        <v>0.5</v>
+        <v>90</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>91</v>
@@ -1232,68 +1217,68 @@
         <v>91</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" ht="NA" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>92</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="n">
+        <v>0.4</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" ht="NA" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="8" t="n">
-        <v>0</v>
+        <v>-0.24</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>145</v>
+        <v>104</v>
+      </c>
+      <c r="D26" s="8" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" ht="NA" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="8" t="n">
-        <v>-0.21</v>
+        <v>0.09</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D27" s="8" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28" ht="NA" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="8" t="n">
-        <v>0.05</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="8" t="n">
-        <v>0.9</v>
+        <v>90</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>91</v>
@@ -1302,82 +1287,82 @@
         <v>91</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" ht="NA" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>92</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="8" t="n">
-        <v>-0.09</v>
+        <v>-0.48</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D31" s="8" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="8" t="n">
-        <v>-0.57</v>
+        <v>-0.27</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D32" s="8" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="8" t="n">
-        <v>-0.35</v>
+        <v>-0.58</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" s="8" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="8" t="n">
-        <v>-0.76</v>
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="8" t="n">
-        <v>0.095</v>
+        <v>90</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="35" ht="NA" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>91</v>
@@ -1386,68 +1371,68 @@
         <v>91</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" ht="NA" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>92</v>
+        <v>35</v>
+      </c>
+      <c r="B36" s="8" t="n">
+        <v>0.44</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>91</v>
+        <v>110</v>
+      </c>
+      <c r="D36" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="37" ht="NA" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="8" t="n">
-        <v>0.58</v>
+        <v>0.69</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D37" s="8" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="38" ht="NA" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="8" t="n">
-        <v>0.44</v>
+        <v>0.33</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D38" s="8" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="39" ht="NA" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="8" t="n">
-        <v>0.32</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="8" t="n">
-        <v>0.6</v>
+        <v>90</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="40" ht="NA" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>91</v>
@@ -1456,40 +1441,40 @@
         <v>91</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" ht="NA" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>92</v>
+        <v>40</v>
+      </c>
+      <c r="B41" s="8" t="n">
+        <v>-0.49</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>91</v>
+        <v>113</v>
+      </c>
+      <c r="D41" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="42" ht="NA" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="8" t="n">
-        <v>-0.21</v>
+        <v>41</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="8" t="n">
-        <v>0.8</v>
+        <v>90</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="43" ht="NA" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>91</v>
@@ -1498,852 +1483,824 @@
         <v>91</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" ht="NA" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>92</v>
+        <v>42</v>
+      </c>
+      <c r="B44" s="8" t="n">
+        <v>0.99</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>91</v>
+        <v>114</v>
+      </c>
+      <c r="D44" s="8" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="45" ht="NA" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="8" t="n">
-        <v>-0.34</v>
+        <v>43</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D45" s="8" t="n">
-        <v>0.8</v>
+        <v>90</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="46" ht="NA" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="8" t="n">
-        <v>1.1</v>
+        <v>39</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D46" s="8" t="n">
-        <v>0.058</v>
+        <v>91</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="47" ht="NA" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>91</v>
+      <c r="B47" s="8" t="n">
+        <v>-0.3</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>91</v>
+        <v>115</v>
+      </c>
+      <c r="D47" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="48" ht="NA" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" ht="NA" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="8" t="n">
-        <v>-0.22</v>
+        <v>46</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="8" t="n">
-        <v>0.4</v>
+        <v>91</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="50" ht="NA" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>91</v>
+        <v>47</v>
+      </c>
+      <c r="B50" s="8" t="n">
+        <v>-0.53</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>91</v>
+        <v>116</v>
+      </c>
+      <c r="D50" s="8" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="51" ht="NA" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>92</v>
+        <v>48</v>
+      </c>
+      <c r="B51" s="8" t="n">
+        <v>0.17</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>91</v>
+        <v>117</v>
+      </c>
+      <c r="D51" s="8" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="52" ht="NA" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="8" t="n">
-        <v>-0.28</v>
+        <v>49</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D52" s="8" t="n">
-        <v>0.8</v>
+        <v>90</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="53" ht="NA" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="8" t="n">
-        <v>0.41</v>
+        <v>50</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D53" s="8" t="n">
-        <v>0.4</v>
+        <v>91</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="54" ht="NA" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="B54" s="8" t="n">
+        <v>0.4</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>91</v>
+        <v>118</v>
+      </c>
+      <c r="D54" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="55" ht="NA" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>92</v>
+        <v>52</v>
+      </c>
+      <c r="B55" s="8" t="n">
+        <v>1.4</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>91</v>
+        <v>119</v>
+      </c>
+      <c r="D55" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="56" ht="NA" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="8" t="n">
-        <v>0.43</v>
+        <v>53</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D56" s="8" t="n">
-        <v>0.4</v>
+        <v>90</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="57" ht="NA" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="8" t="n">
-        <v>1.8</v>
+        <v>54</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" s="8" t="n">
-        <v>0.2</v>
+        <v>91</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="58" ht="NA" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>91</v>
+        <v>55</v>
+      </c>
+      <c r="B58" s="8" t="n">
+        <v>0.52</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>91</v>
+        <v>120</v>
+      </c>
+      <c r="D58" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="59" ht="NA" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>92</v>
+        <v>56</v>
+      </c>
+      <c r="B59" s="8" t="n">
+        <v>1.1</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>91</v>
+        <v>121</v>
+      </c>
+      <c r="D59" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="60" ht="NA" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="8" t="n">
-        <v>0.46</v>
+        <v>57</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D60" s="8" t="n">
-        <v>0.6</v>
+        <v>90</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="61" ht="NA" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="8" t="n">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D61" s="8" t="n">
-        <v>0.2</v>
+        <v>91</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="62" ht="NA" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>91</v>
+      <c r="B62" s="8" t="n">
+        <v>0.26</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>91</v>
+        <v>122</v>
+      </c>
+      <c r="D62" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" ht="NA" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>92</v>
+        <v>59</v>
+      </c>
+      <c r="B63" s="8" t="n">
+        <v>2.3</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>91</v>
+        <v>123</v>
+      </c>
+      <c r="D63" s="8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="64" ht="NA" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64" s="8" t="n">
-        <v>0.33</v>
+        <v>0.69</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D64" s="8" t="n">
-        <v>0.2</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="65" ht="NA" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="8" t="n">
-        <v>2.5</v>
+        <v>61</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="8" t="n">
-        <v>0.14</v>
+        <v>90</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="66" ht="NA" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" s="8" t="n">
-        <v>0.73</v>
+        <v>62</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D66" s="8" t="n">
-        <v>0.013</v>
+        <v>91</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="67" ht="NA" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>91</v>
+        <v>63</v>
+      </c>
+      <c r="B67" s="8" t="n">
+        <v>1.6</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>91</v>
+        <v>125</v>
+      </c>
+      <c r="D67" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="68" ht="NA" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>92</v>
+        <v>64</v>
+      </c>
+      <c r="B68" s="8" t="n">
+        <v>-1.7</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>91</v>
+        <v>126</v>
+      </c>
+      <c r="D68" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="69" ht="NA" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B69" s="8" t="n">
-        <v>1.9</v>
+        <v>-2.5</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D69" s="8" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="70" ht="NA" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B70" s="8" t="n">
-        <v>-1.7</v>
+        <v>-2.9</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D70" s="8" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="71" ht="NA" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="8" t="n">
-        <v>-2.3</v>
+        <v>67</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D71" s="8" t="n">
-        <v>0.3</v>
+        <v>90</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="72" ht="NA" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" s="8" t="n">
-        <v>-2.7</v>
+        <v>68</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D72" s="8" t="n">
-        <v>0.2</v>
+        <v>91</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="73" ht="NA" customHeight="1">
       <c r="A73" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>91</v>
+        <v>69</v>
+      </c>
+      <c r="B73" s="8" t="n">
+        <v>0.45</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>91</v>
+        <v>129</v>
+      </c>
+      <c r="D73" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="74" ht="NA" customHeight="1">
       <c r="A74" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" ht="NA" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" s="8" t="n">
-        <v>0.46</v>
+        <v>68</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D75" s="8" t="n">
-        <v>0.3</v>
+        <v>91</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="76" ht="NA" customHeight="1">
       <c r="A76" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B76" s="8" t="s">
-        <v>91</v>
+      <c r="B76" s="8" t="n">
+        <v>-0.24</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>91</v>
+        <v>130</v>
+      </c>
+      <c r="D76" s="8" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="77" ht="NA" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" ht="NA" customHeight="1">
       <c r="A78" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B78" s="8" t="n">
-        <v>-0.25</v>
+        <v>68</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D78" s="8" t="n">
-        <v>0.5</v>
+        <v>91</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="79" ht="NA" customHeight="1">
       <c r="A79" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>91</v>
+      <c r="B79" s="8" t="n">
+        <v>0.29</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>91</v>
+        <v>131</v>
+      </c>
+      <c r="D79" s="8" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" ht="NA" customHeight="1">
       <c r="A80" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" ht="NA" customHeight="1">
       <c r="A81" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B81" s="8" t="n">
-        <v>0.22</v>
+        <v>68</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D81" s="8" t="n">
-        <v>0.7</v>
+        <v>91</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="82" ht="NA" customHeight="1">
       <c r="A82" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>91</v>
+      <c r="B82" s="8" t="n">
+        <v>0.96</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>91</v>
+        <v>132</v>
+      </c>
+      <c r="D82" s="8" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="83" ht="NA" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" ht="NA" customHeight="1">
       <c r="A84" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B84" s="8" t="n">
-        <v>0.76</v>
+        <v>68</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D84" s="8" t="n">
-        <v>0.023</v>
+        <v>91</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="85" ht="NA" customHeight="1">
       <c r="A85" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>91</v>
+      <c r="B85" s="8" t="n">
+        <v>0.52</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>91</v>
+        <v>133</v>
+      </c>
+      <c r="D85" s="8" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="86" ht="NA" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" ht="NA" customHeight="1">
       <c r="A87" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="8" t="n">
-        <v>0.55</v>
+        <v>68</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D87" s="8" t="n">
-        <v>0.3</v>
+        <v>91</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="88" ht="NA" customHeight="1">
       <c r="A88" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>91</v>
+      <c r="B88" s="8" t="n">
+        <v>0.14</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>91</v>
+        <v>134</v>
+      </c>
+      <c r="D88" s="8" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="89" ht="NA" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" ht="NA" customHeight="1">
       <c r="A90" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B90" s="8" t="n">
-        <v>0.26</v>
+        <v>68</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D90" s="8" t="n">
-        <v>0.4</v>
+        <v>91</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="91" ht="NA" customHeight="1">
       <c r="A91" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>91</v>
+      <c r="B91" s="8" t="n">
+        <v>0.82</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>91</v>
+        <v>135</v>
+      </c>
+      <c r="D91" s="8" t="n">
+        <v>0.006</v>
       </c>
     </row>
     <row r="92" ht="NA" customHeight="1">
       <c r="A92" s="3" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" ht="NA" customHeight="1">
       <c r="A93" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B93" s="8" t="n">
-        <v>0.81</v>
+        <v>68</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D93" s="8" t="n">
-        <v>0.005</v>
+        <v>91</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="94" ht="NA" customHeight="1">
       <c r="A94" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>91</v>
+      <c r="B94" s="8" t="n">
+        <v>0.4</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>91</v>
+        <v>136</v>
+      </c>
+      <c r="D94" s="8" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="95" ht="NA" customHeight="1">
       <c r="A95" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" ht="NA" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B96" s="8" t="n">
-        <v>0.48</v>
+        <v>68</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D96" s="8" t="n">
-        <v>0.3</v>
+        <v>91</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="97" ht="NA" customHeight="1">
       <c r="A97" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>91</v>
+      <c r="B97" s="8" t="n">
+        <v>0.52</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>91</v>
+        <v>137</v>
+      </c>
+      <c r="D97" s="8" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="98" ht="NA" customHeight="1">
       <c r="A98" s="3" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" ht="NA" customHeight="1">
       <c r="A99" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B99" s="8" t="n">
-        <v>0.59</v>
+        <v>68</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D99" s="8" t="n">
-        <v>0.052</v>
+        <v>91</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="100" ht="NA" customHeight="1">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B100" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>91</v>
+      <c r="B100" s="9" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D100" s="9" t="n">
+        <v>0.005</v>
       </c>
     </row>
     <row r="101" ht="NA" customHeight="1">
-      <c r="A101" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="102" ht="NA" customHeight="1">
-      <c r="A102" s="4" t="s">
+      <c r="A101" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B102" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D102" s="9" t="n">
-        <v>0.071</v>
-      </c>
-    </row>
-    <row r="103" ht="NA" customHeight="1">
-      <c r="A103" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>89</v>
+      <c r="B101" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A101:D101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>